<commit_message>
Rename to Business Documentation - Only one KPI to do now
</commit_message>
<xml_diff>
--- a/Business/AanrijdingData.xlsx
+++ b/Business/AanrijdingData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weilin\Desktop\School\Proftaak\proftaak22\Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BE64A18-389C-4301-8B96-DF2A1ACC3A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011E2A88-51C3-4CBC-94B3-5329D8F4B73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="28145" windowHeight="17062" xr2:uid="{6DE98BD3-8520-4AAB-B20E-7714066C886F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Perioden</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>DMV_aanrijding_of_object_op_spoor</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F8A98D-ED85-4723-BC8B-AF90F3491C59}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.3"/>
@@ -408,7 +411,7 @@
     <col min="3" max="3" width="18.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,8 +421,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -427,11 +433,14 @@
         <v>1846</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C5" si="0">B2/100*14.60017735</f>
-        <v>269.519273881</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+      <c r="F2">
+        <f>C2/B2*100</f>
+        <v>15.872156013001085</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2012</v>
       </c>
@@ -439,11 +448,14 @@
         <v>2074</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" si="0"/>
-        <v>302.80767823899998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F12" si="0">C3/B3*100</f>
+        <v>15.766634522661525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2013</v>
       </c>
@@ -451,11 +463,14 @@
         <v>2312</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>337.55610033199997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>14.316608996539792</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2014</v>
       </c>
@@ -463,11 +478,14 @@
         <v>2484</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>362.66840537399997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>11.674718196457327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -475,11 +493,14 @@
         <v>2947</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C12" si="1">B6/100*14.60017735</f>
-        <v>430.26722650449994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>13.403461146929081</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2016</v>
       </c>
@@ -487,11 +508,14 @@
         <v>3031</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
-        <v>442.53137547849997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>12.30616958099637</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2017</v>
       </c>
@@ -499,11 +523,14 @@
         <v>4085</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
-        <v>596.41724474750004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>11.946144430844553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -511,11 +538,14 @@
         <v>5190</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="1"/>
-        <v>757.74920446499993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>10.038535645472061</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -523,11 +553,14 @@
         <v>6000</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="1"/>
-        <v>876.01064099999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>641</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>10.683333333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -535,11 +568,15 @@
         <v>4450</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C11:C12" si="1">B11/100*14.60017735</f>
         <v>649.70789207500002</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>14.600177350000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -549,6 +586,10 @@
       <c r="C12" s="1">
         <f t="shared" si="1"/>
         <v>581.52506385049992</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>14.600177349999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>